<commit_message>
WIred data blocks to IDEX
</commit_message>
<xml_diff>
--- a/Competition/AssemblyToBinary.xlsx
+++ b/Competition/AssemblyToBinary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrine\VivadoProjects\ECE369AryDavidRusty\Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5034EF0-6CB4-4706-A759-309C8A93E730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8B3F4E-76A6-4D3D-8688-A6080C36A52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="131">
   <si>
     <t>20107fff</t>
   </si>
@@ -192,18 +192,6 @@
     <t>sll</t>
   </si>
   <si>
-    <t>$s3, $s1, 6 -&gt;</t>
-  </si>
-  <si>
-    <t>$s3, $s1, 6</t>
-  </si>
-  <si>
-    <t>$t9, $s2, 4 -&gt;</t>
-  </si>
-  <si>
-    <t>$t9, $s2, 4</t>
-  </si>
-  <si>
     <t>$s3, $s3, $t9 -&gt;</t>
   </si>
   <si>
@@ -369,12 +357,6 @@
     <t>00005020</t>
   </si>
   <si>
-    <t>00119980</t>
-  </si>
-  <si>
-    <t>22590004</t>
-  </si>
-  <si>
     <t>02799820</t>
   </si>
   <si>
@@ -400,6 +382,42 @@
   </si>
   <si>
     <t>lwf</t>
+  </si>
+  <si>
+    <t>010010</t>
+  </si>
+  <si>
+    <t>00119a00</t>
+  </si>
+  <si>
+    <t>$s3, $s1, 8 -&gt;</t>
+  </si>
+  <si>
+    <t>$s3, $s1, 8</t>
+  </si>
+  <si>
+    <t>22590010</t>
+  </si>
+  <si>
+    <t>$t9, $s2, 16 -&gt;</t>
+  </si>
+  <si>
+    <t>$t9, $s2, 16</t>
+  </si>
+  <si>
+    <t>lwv</t>
+  </si>
+  <si>
+    <t>$s3</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>0000000000000000</t>
+  </si>
+  <si>
+    <t>4a600000</t>
   </si>
 </sst>
 </file>
@@ -718,15 +736,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -757,7 +776,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -777,7 +796,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -823,7 +842,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -843,7 +862,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1067,9 +1086,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -1078,63 +1097,84 @@
         <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="I17" t="s">
         <v>54</v>
       </c>
       <c r="J17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="1">
+        <v>10011</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="I18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -1143,130 +1183,130 @@
         <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I21" t="s">
         <v>18</v>
       </c>
       <c r="J21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E23" t="s">
         <v>66</v>
       </c>
-      <c r="I22" t="s">
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
         <v>65</v>
       </c>
-      <c r="J22" t="s">
+      <c r="H23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
         <v>68</v>
       </c>
-      <c r="D23" t="s">
+      <c r="I24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" t="s">
         <v>69</v>
       </c>
-      <c r="E23" t="s">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
         <v>70</v>
       </c>
-      <c r="F23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I25" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>77</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I26" t="s">
         <v>12</v>
       </c>
       <c r="J26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -1275,18 +1315,18 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
         <v>15</v>
       </c>
       <c r="J27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -1295,18 +1335,18 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I28" t="s">
         <v>3</v>
       </c>
       <c r="J28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -1315,56 +1355,56 @@
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I29" t="s">
         <v>48</v>
       </c>
       <c r="J29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
         <v>87</v>
       </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
         <v>88</v>
       </c>
-      <c r="I30" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" t="s">
-        <v>91</v>
-      </c>
-      <c r="I31" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -1426,7 +1466,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1435,13 +1475,13 @@
         <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I35" t="s">
         <v>31</v>
       </c>
       <c r="J35" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -1472,27 +1512,27 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
         <v>15</v>
       </c>
       <c r="H37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -1501,18 +1541,18 @@
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I38" t="s">
         <v>3</v>
       </c>
       <c r="J38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -1521,13 +1561,13 @@
         <v>48</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I39" t="s">
         <v>48</v>
       </c>
       <c r="J39" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -1552,7 +1592,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -1561,18 +1601,18 @@
         <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="I41" t="s">
         <v>54</v>
       </c>
       <c r="J41" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -1581,43 +1621,46 @@
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="I42" t="s">
         <v>3</v>
       </c>
       <c r="J42" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
-        <v>124</v>
+      <c r="A43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" t="s">
-        <v>59</v>
-      </c>
-      <c r="I44" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" t="s">
-        <v>60</v>
+        <v>130</v>
+      </c>
+      <c r="D44" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -1626,64 +1669,64 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I45" t="s">
         <v>18</v>
       </c>
       <c r="J45" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J46" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E47" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G47" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -1692,33 +1735,73 @@
         <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I48" t="s">
         <v>3</v>
       </c>
       <c r="J48" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F49" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I49" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J49" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" t="s">
+        <v>3</v>
+      </c>
+      <c r="J50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" t="s">
+        <v>104</v>
+      </c>
+      <c r="I51" t="s">
+        <v>61</v>
+      </c>
+      <c r="J51" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Memory block reading
</commit_message>
<xml_diff>
--- a/Competition/AssemblyToBinary.xlsx
+++ b/Competition/AssemblyToBinary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrine\VivadoProjects\ECE369AryDavidRusty\Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8B3F4E-76A6-4D3D-8688-A6080C36A52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961C9E91-2D36-4889-80DB-4025DE07E4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="135">
   <si>
     <t>20107fff</t>
   </si>
@@ -387,24 +387,6 @@
     <t>010010</t>
   </si>
   <si>
-    <t>00119a00</t>
-  </si>
-  <si>
-    <t>$s3, $s1, 8 -&gt;</t>
-  </si>
-  <si>
-    <t>$s3, $s1, 8</t>
-  </si>
-  <si>
-    <t>22590010</t>
-  </si>
-  <si>
-    <t>$t9, $s2, 16 -&gt;</t>
-  </si>
-  <si>
-    <t>$t9, $s2, 16</t>
-  </si>
-  <si>
     <t>lwv</t>
   </si>
   <si>
@@ -418,6 +400,36 @@
   </si>
   <si>
     <t>4a600000</t>
+  </si>
+  <si>
+    <t>001199c0</t>
+  </si>
+  <si>
+    <t>$s3, $s1, 7 -&gt;</t>
+  </si>
+  <si>
+    <t>$s3, $s1, 7</t>
+  </si>
+  <si>
+    <t>22590008</t>
+  </si>
+  <si>
+    <t>$t9, $s2, 8 -&gt;</t>
+  </si>
+  <si>
+    <t>$t9, $s2, 8</t>
+  </si>
+  <si>
+    <t>lww</t>
+  </si>
+  <si>
+    <t>010011</t>
+  </si>
+  <si>
+    <t>0010 0000 0000 1000</t>
+  </si>
+  <si>
+    <t>4c002008</t>
   </si>
 </sst>
 </file>
@@ -736,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,7 +760,7 @@
     <col min="14" max="14" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>106</v>
       </c>
@@ -794,7 +806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>107</v>
       </c>
@@ -814,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -840,129 +852,129 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>15</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="I8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -971,18 +983,18 @@
         <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
       </c>
       <c r="J11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -991,402 +1003,402 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I12" t="s">
         <v>31</v>
       </c>
       <c r="J12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>41</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>15</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="I14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>49</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
         <v>48</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="J17" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I18" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="J18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>129</v>
+      </c>
       <c r="I19" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>130</v>
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="K20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L20" s="1">
-        <v>10011</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O20" s="1"/>
+      <c r="I20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" t="s">
-        <v>59</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L21" s="1">
+        <v>10011</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="J22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
-      </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="I23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I26" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="J26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I29" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I30" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="J30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -1395,18 +1407,18 @@
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I31" t="s">
         <v>3</v>
       </c>
       <c r="J31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -1415,18 +1427,18 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="I32" t="s">
         <v>3</v>
       </c>
       <c r="J32" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
@@ -1435,38 +1447,38 @@
         <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I33" t="s">
         <v>3</v>
       </c>
       <c r="J33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I34" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="J34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1475,18 +1487,18 @@
         <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="I35" t="s">
         <v>31</v>
       </c>
       <c r="J35" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -1495,312 +1507,332 @@
         <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="I36" t="s">
         <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
       <c r="E37" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" t="s">
-        <v>94</v>
+        <v>38</v>
+      </c>
+      <c r="I37" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
-      </c>
-      <c r="I38" t="s">
-        <v>3</v>
-      </c>
-      <c r="J38" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I39" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="J39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F40" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="I40" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J40" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="I41" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="J41" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I42" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="J42" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="I43" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J43" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D44" t="s">
-        <v>126</v>
+        <v>110</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" t="s">
-        <v>58</v>
-      </c>
-      <c r="I45" t="s">
-        <v>18</v>
-      </c>
-      <c r="J45" t="s">
-        <v>59</v>
+        <v>124</v>
+      </c>
+      <c r="D45" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F46" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="I46" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="J46" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C47" t="s">
-        <v>103</v>
-      </c>
-      <c r="D47" t="s">
-        <v>65</v>
-      </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F47" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47" t="s">
-        <v>65</v>
-      </c>
-      <c r="H47" t="s">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="I47" t="s">
+        <v>61</v>
+      </c>
+      <c r="J47" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
       </c>
+      <c r="C48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
       <c r="E48" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="F48" t="s">
-        <v>68</v>
-      </c>
-      <c r="I48" t="s">
-        <v>3</v>
-      </c>
-      <c r="J48" t="s">
-        <v>69</v>
+        <v>103</v>
+      </c>
+      <c r="G48" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="I49" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="J49" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="I50" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="J50" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
         <v>61</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>104</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>61</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J52" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lww and lvw should be working
</commit_message>
<xml_diff>
--- a/Competition/AssemblyToBinary.xlsx
+++ b/Competition/AssemblyToBinary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrine\VivadoProjects\ECE369AryDavidRusty\Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961C9E91-2D36-4889-80DB-4025DE07E4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244CC7A2-FDDB-42B2-8E52-5FFFA06D7861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4872" yWindow="3372" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="140">
   <si>
     <t>20107fff</t>
   </si>
@@ -430,6 +430,21 @@
   </si>
   <si>
     <t>4c002008</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>$s4</t>
+  </si>
+  <si>
+    <t>10100</t>
+  </si>
+  <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>4400a000</t>
   </si>
 </sst>
 </file>
@@ -748,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -892,49 +907,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -943,18 +938,18 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I9" t="s">
         <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -963,38 +958,38 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10" t="s">
         <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1003,18 +998,18 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I12" t="s">
         <v>31</v>
       </c>
       <c r="J12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1023,482 +1018,482 @@
         <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I13" t="s">
         <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I16" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="I18" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I19" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="J19" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>129</v>
+      </c>
       <c r="I20" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>124</v>
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="K21" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L21" s="1">
-        <v>10011</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O21" s="1"/>
+      <c r="I21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" t="s">
-        <v>59</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="K22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L22" s="1">
+        <v>10011</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" t="s">
-        <v>65</v>
-      </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="I24" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="J26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I27" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="J27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="G28" t="s">
+        <v>73</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="J30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I31" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="J31" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
         <v>87</v>
       </c>
-      <c r="I32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
         <v>25</v>
       </c>
-      <c r="I33" t="s">
-        <v>3</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="I34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>3</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
         <v>28</v>
       </c>
-      <c r="I34" t="s">
-        <v>3</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="I35" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I35" t="s">
-        <v>31</v>
-      </c>
-      <c r="J35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -1507,18 +1502,18 @@
         <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="I36" t="s">
         <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -1527,273 +1522,282 @@
         <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="I37" t="s">
         <v>31</v>
       </c>
       <c r="J37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I38" t="s">
+        <v>31</v>
+      </c>
+      <c r="J38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>92</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>15</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>93</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>92</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>15</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
         <v>96</v>
       </c>
-      <c r="I39" t="s">
-        <v>3</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="I40" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B40" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
         <v>48</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>99</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I41" t="s">
         <v>48</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J41" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>18</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>52</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I42" t="s">
         <v>18</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>54</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>126</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I43" t="s">
         <v>54</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J43" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
         <v>129</v>
       </c>
-      <c r="I43" t="s">
-        <v>3</v>
-      </c>
-      <c r="J43" t="s">
+      <c r="I44" t="s">
+        <v>3</v>
+      </c>
+      <c r="J44" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
         <v>18</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>55</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>18</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
         <v>18</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>58</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>18</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>61</v>
-      </c>
-      <c r="F47" t="s">
-        <v>101</v>
-      </c>
-      <c r="I47" t="s">
-        <v>61</v>
-      </c>
-      <c r="J47" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>103</v>
-      </c>
-      <c r="D48" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="E48" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="F48" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48" t="s">
-        <v>65</v>
-      </c>
-      <c r="H48" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="K48" s="1">
+        <v>10001</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="F49" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="I49" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="J49" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
       <c r="E50" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F50" t="s">
-        <v>104</v>
-      </c>
-      <c r="I50" t="s">
-        <v>61</v>
-      </c>
-      <c r="J50" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="G50" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -1833,6 +1837,46 @@
         <v>61</v>
       </c>
       <c r="J52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>68</v>
+      </c>
+      <c r="I53" t="s">
+        <v>3</v>
+      </c>
+      <c r="J53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" t="s">
+        <v>104</v>
+      </c>
+      <c r="I54" t="s">
+        <v>61</v>
+      </c>
+      <c r="J54" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>